<commit_message>
adding import-gbx to the menu
</commit_message>
<xml_diff>
--- a/docs/en/assets/demo-portfolio-03-calculation.xlsx
+++ b/docs/en/assets/demo-portfolio-03-calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8b4af0312c2de9c5/Projects/PortfolioPerformance/portfolio-help/docs/en/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1182" documentId="8_{6835218D-69E8-464C-AC23-083D53515D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64B4F23B-8CC5-4154-8E4D-37CA4F674A44}"/>
+  <xr:revisionPtr revIDLastSave="1256" documentId="8_{6835218D-69E8-464C-AC23-083D53515D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71D4D8CA-A740-48D6-A0E3-9990BE38A6C9}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="3590" windowWidth="18940" windowHeight="15590" tabRatio="709" firstSheet="7" activeTab="10" xr2:uid="{F6198169-F7A1-41B8-ADFA-DF561FC496C5}"/>
+    <workbookView xWindow="230" yWindow="2420" windowWidth="19860" windowHeight="15590" tabRatio="709" firstSheet="7" activeTab="10" xr2:uid="{F6198169-F7A1-41B8-ADFA-DF561FC496C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Export-entire-portfolio-raw" sheetId="12" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="129">
   <si>
     <t>XIRR</t>
   </si>
@@ -405,16 +405,7 @@
     <t>… To</t>
   </si>
   <si>
-    <t>1st Buy</t>
-  </si>
-  <si>
-    <t>2nd Buy</t>
-  </si>
-  <si>
     <t>HP4</t>
-  </si>
-  <si>
-    <t>dividend</t>
   </si>
   <si>
     <t>(J3*J4*J5*J6)-1</t>
@@ -459,17 +450,28 @@
     <t>HP5</t>
   </si>
   <si>
-    <t>End reporting</t>
+    <t>start --&gt;  1st Buy</t>
+  </si>
+  <si>
+    <t>1st buy --&gt; 2nd Buy</t>
+  </si>
+  <si>
+    <t>2nd buy --&gt; dividend</t>
+  </si>
+  <si>
+    <t>dividend --&gt; sell</t>
+  </si>
+  <si>
+    <t>sell --&gt; End</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$EUR]\ #,##0.00;[$EUR]\ \-#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -894,7 +896,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1111,6 +1113,9 @@
     <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1151,10 +1156,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1919,59 +1920,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>500063</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>500063</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>178594</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Straight Arrow Connector 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EF4DEE8-38A6-4CC4-9223-2F4134DAA2D3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3465513" y="927100"/>
-          <a:ext cx="0" cy="203994"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
@@ -2410,7 +2358,7 @@
         <v>33</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G1" s="69" t="s">
         <v>63</v>
@@ -31395,15 +31343,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="112" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="113"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="114"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" s="80" t="s">
@@ -31416,10 +31364,10 @@
         <v>54</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>67</v>
@@ -31513,7 +31461,7 @@
       <c r="A7" s="82"/>
       <c r="B7" s="1"/>
       <c r="F7" s="93" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G7" s="84"/>
     </row>
@@ -31531,7 +31479,7 @@
         <v>0.44162138823750774</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G9" s="86"/>
     </row>
@@ -31547,7 +31495,7 @@
       </c>
       <c r="E10" s="89"/>
       <c r="F10" s="91" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G10" s="92"/>
     </row>
@@ -31562,35 +31510,38 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F23F1A-FC8C-4B96-898D-0E104FDB01D2}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
-    <col min="3" max="4" width="12.36328125" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="111" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="112" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="113"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="114"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>105</v>
       </c>
@@ -31605,13 +31556,13 @@
         <v>54</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G2" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>117</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>120</v>
       </c>
       <c r="I2" s="21" t="s">
         <v>67</v>
@@ -31620,203 +31571,179 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="50" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="1">
-        <v>44211</v>
+        <v>43994</v>
       </c>
       <c r="C3" s="1">
-        <v>44574</v>
+        <v>44210</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>160.26</v>
-      </c>
-      <c r="G3">
-        <v>153</v>
-      </c>
-      <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" s="83">
-        <f>((F3)/(E3+G3-H3))-1</f>
-        <v>4.7450980392156783E-2</v>
+        <v>0</v>
       </c>
       <c r="J3" s="84">
-        <f>1+I3</f>
-        <v>1.0474509803921568</v>
-      </c>
-      <c r="K3" s="2">
-        <f>J3-1</f>
-        <v>4.7450980392156783E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="50" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="1">
-        <v>44575</v>
+        <v>44211</v>
       </c>
       <c r="C4" s="1">
-        <v>44909</v>
+        <v>44574</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="E4">
+        <v>150.5</v>
+      </c>
+      <c r="F4">
         <v>160.26</v>
       </c>
-      <c r="F4">
-        <v>239.43</v>
-      </c>
       <c r="G4">
-        <v>83</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="I4" s="83">
-        <f t="shared" ref="I4:I7" si="0">((F4)/(E4+G4-H4))-1</f>
-        <v>-1.5744470936446486E-2</v>
+        <f>((F4)/(E4+G4-H4))-1</f>
+        <v>-0.47196046128500824</v>
       </c>
       <c r="J4" s="84">
-        <f t="shared" ref="J4:J7" si="1">1+I4</f>
-        <v>0.98425552906355351</v>
-      </c>
-      <c r="K4" s="114">
-        <f>(J3*J4)-1</f>
-        <v>3.0959418874020095E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <f>1+I4</f>
+        <v>0.52803953871499176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="50" t="s">
         <v>104</v>
       </c>
       <c r="B5" s="1">
-        <v>44910</v>
+        <v>44575</v>
       </c>
       <c r="C5" s="1">
-        <v>45027</v>
+        <v>44909</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="E5">
         <f>F4</f>
-        <v>239.43</v>
+        <v>160.26</v>
       </c>
       <c r="F5">
-        <v>283.47000000000003</v>
-      </c>
-      <c r="H5">
-        <v>30</v>
+        <v>287.49</v>
+      </c>
+      <c r="G5">
+        <v>83</v>
       </c>
       <c r="I5" s="83">
-        <f t="shared" si="0"/>
-        <v>0.35353101274888998</v>
+        <f t="shared" ref="I5:I7" si="0">((F5)/(E5+G5-H5))-1</f>
+        <v>0.18182191893447341</v>
       </c>
       <c r="J5" s="84">
-        <f t="shared" si="1"/>
-        <v>1.35353101274889</v>
-      </c>
-      <c r="K5" s="114">
-        <f>(J3*J4*J5)-1</f>
-        <v>0.39543554633155953</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <f t="shared" ref="J5:J7" si="1">1+I5</f>
+        <v>1.1818219189344734</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="50" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1">
-        <v>45028</v>
+        <v>44910</v>
       </c>
       <c r="C6" s="1">
-        <v>45028</v>
+        <v>45027</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="E6">
         <f>F5</f>
-        <v>283.47000000000003</v>
+        <v>287.49</v>
       </c>
       <c r="F6">
-        <v>224</v>
+        <v>339</v>
       </c>
       <c r="H6">
-        <v>107</v>
+        <v>30</v>
       </c>
       <c r="I6" s="83">
         <f t="shared" si="0"/>
-        <v>0.26933756445854806</v>
+        <v>0.31655598275661179</v>
       </c>
       <c r="J6" s="84">
         <f t="shared" si="1"/>
-        <v>1.2693375644585481</v>
-      </c>
-      <c r="K6" s="114">
-        <f>(J3*J4*J5*J6)-1</f>
-        <v>0.77127875773938515</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="115" t="s">
-        <v>126</v>
+        <v>1.3165559827566118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="100" t="s">
+        <v>123</v>
       </c>
       <c r="B7" s="1">
-        <v>45029</v>
+        <v>45028</v>
       </c>
       <c r="C7" s="1">
         <v>45089</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E7">
         <f>F6</f>
-        <v>224</v>
+        <v>339</v>
       </c>
       <c r="F7">
         <v>190.06</v>
       </c>
+      <c r="H7">
+        <v>107</v>
+      </c>
       <c r="I7" s="83">
         <f t="shared" si="0"/>
-        <v>-0.15151785714285715</v>
+        <v>-0.18077586206896545</v>
       </c>
       <c r="J7" s="84">
         <f t="shared" si="1"/>
-        <v>0.84848214285714285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>0.81922413793103455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="82"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="J8" s="84"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="85"/>
       <c r="I9" s="93" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J9" s="86"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="85"/>
       <c r="I10" s="93"/>
       <c r="J10" s="86"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="87" t="s">
         <v>69</v>
       </c>
@@ -31825,14 +31752,14 @@
       <c r="D11" s="72"/>
       <c r="F11" s="83">
         <f>(J3*J4*J5*J6*J7)-1</f>
-        <v>0.50289839596405161</v>
+        <v>-0.32692950284195754</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J11" s="86"/>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="88" t="s">
         <v>70</v>
       </c>
@@ -31842,12 +31769,12 @@
       <c r="E12" s="89"/>
       <c r="F12" s="90">
         <f>GEOMEAN(J3:J6)-1</f>
-        <v>0.15364377924156236</v>
+        <v>-4.7939704972544295E-2</v>
       </c>
       <c r="G12" s="89"/>
       <c r="H12" s="89"/>
       <c r="I12" s="91" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J12" s="92"/>
     </row>
@@ -31878,19 +31805,19 @@
         <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
         <v>117</v>
-      </c>
-      <c r="E1" t="s">
-        <v>120</v>
       </c>
       <c r="F1" t="s">
         <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -58419,10 +58346,10 @@
     </row>
     <row r="1102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D1102" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F1102" s="96" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="1106" spans="1:6" x14ac:dyDescent="0.35">
@@ -58922,21 +58849,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="F2" s="101" t="s">
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="F2" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="J2" s="101" t="s">
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="J2" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -59170,8 +59097,8 @@
       <c r="D15" s="1"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="100"/>
-      <c r="C17" s="100"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="101"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="1"/>
@@ -59182,8 +59109,8 @@
       <c r="L19" s="9"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="102"/>
-      <c r="C20" s="102"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="103"/>
       <c r="E20" s="2"/>
       <c r="L20" s="9"/>
     </row>
@@ -59191,8 +59118,8 @@
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="100"/>
-      <c r="C22" s="100"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="101"/>
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
@@ -59208,8 +59135,8 @@
       <c r="L26" s="9"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="100"/>
-      <c r="C27" s="100"/>
+      <c r="B27" s="101"/>
+      <c r="C27" s="101"/>
       <c r="L27" s="9"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
@@ -59238,8 +59165,8 @@
       <c r="N35" s="13"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B36" s="100"/>
-      <c r="C36" s="100"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="101"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B37" s="1"/>
@@ -59302,22 +59229,22 @@
       <c r="B2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="103"/>
+      <c r="D2" s="104"/>
       <c r="E2" s="4"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="103" t="s">
+      <c r="H2" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="103"/>
+      <c r="I2" s="104"/>
     </row>
     <row r="3" spans="2:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="105" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="16">
@@ -59326,7 +59253,7 @@
       <c r="D3">
         <v>77.5</v>
       </c>
-      <c r="G3" s="104" t="s">
+      <c r="G3" s="105" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="1">
@@ -59337,14 +59264,14 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="105"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="16">
         <v>45028</v>
       </c>
       <c r="D4">
         <v>105</v>
       </c>
-      <c r="G4" s="105"/>
+      <c r="G4" s="106"/>
       <c r="H4" s="1">
         <v>45089</v>
       </c>
@@ -59354,8 +59281,8 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C5" s="106"/>
-      <c r="D5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="108"/>
       <c r="E5" s="6"/>
       <c r="I5" s="5"/>
       <c r="L5" s="62">
@@ -59396,10 +59323,10 @@
       <c r="B12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="103"/>
+      <c r="D12" s="104"/>
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
@@ -59562,42 +59489,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.5">
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="111"/>
     </row>
     <row r="3" spans="2:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
       <c r="E3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
       <c r="I3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="101" t="s">
+      <c r="J3" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
       <c r="M3" s="18" t="s">
         <v>29</v>
       </c>
@@ -59818,36 +59745,36 @@
       </c>
     </row>
     <row r="12" spans="2:13" ht="21" x14ac:dyDescent="0.5">
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109"/>
-      <c r="J12" s="109"/>
-      <c r="K12" s="109"/>
-      <c r="L12" s="110"/>
+      <c r="C12" s="110"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="110"/>
+      <c r="G12" s="110"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
+      <c r="J12" s="110"/>
+      <c r="K12" s="110"/>
+      <c r="L12" s="111"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B13" s="101" t="s">
+      <c r="B13" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="F13" s="101" t="s">
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="F13" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101"/>
-      <c r="J13" s="101" t="s">
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="J13" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="101"/>
-      <c r="L13" s="101"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14" t="s">

</xml_diff>